<commit_message>
Add explanation for variables, change city names, change template
</commit_message>
<xml_diff>
--- a/devdata/Data.xlsx
+++ b/devdata/Data.xlsx
@@ -40,7 +40,7 @@
     <t>4 Service Center</t>
   </si>
   <si>
-    <t>Ladário</t>
+    <t>Toronto</t>
   </si>
   <si>
     <t>2019/07/03</t>
@@ -58,7 +58,7 @@
     <t>197 Ronald Regan Drive</t>
   </si>
   <si>
-    <t>Corpus</t>
+    <t>New York</t>
   </si>
   <si>
     <t>2019/05/03</t>
@@ -76,7 +76,7 @@
     <t>3554 Chive Circle</t>
   </si>
   <si>
-    <t>Manggissari</t>
+    <t>San Francisco</t>
   </si>
   <si>
     <t>2019/05/10</t>
@@ -94,7 +94,7 @@
     <t>20533 6th Crossing</t>
   </si>
   <si>
-    <t>Kebonagung</t>
+    <t>Milan</t>
   </si>
   <si>
     <t>2019/12/14</t>
@@ -112,7 +112,7 @@
     <t>9 Michigan Street</t>
   </si>
   <si>
-    <t>Kalynivka</t>
+    <t>Kansas City</t>
   </si>
   <si>
     <t>2020/02/12</t>
@@ -130,7 +130,7 @@
     <t>8 Grim Trail</t>
   </si>
   <si>
-    <t>Fonte da Aldeia</t>
+    <t>Lahore</t>
   </si>
   <si>
     <t>2019/05/05</t>
@@ -148,7 +148,7 @@
     <t>91764 Reindahl Park</t>
   </si>
   <si>
-    <t>Troitskoye</t>
+    <t>New Dehli</t>
   </si>
   <si>
     <t>2019/12/17</t>
@@ -166,7 +166,7 @@
     <t>8077 Pennsylvania Drive</t>
   </si>
   <si>
-    <t>Muesanaik</t>
+    <t>Helsinki</t>
   </si>
   <si>
     <t>2020/02/09</t>
@@ -184,7 +184,7 @@
     <t>3619 Oxford Place</t>
   </si>
   <si>
-    <t>Matou</t>
+    <t>Stockholm</t>
   </si>
   <si>
     <t>2019/10/30</t>
@@ -202,7 +202,7 @@
     <t>4 Cambridge Center</t>
   </si>
   <si>
-    <t>Verbilki</t>
+    <t>London</t>
   </si>
   <si>
     <t>2020/03/26</t>
@@ -235,12 +235,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -253,16 +259,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -279,7 +285,7 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -299,6 +305,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -437,13 +444,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -542,10 +543,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -800,13 +801,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1119,10 +1114,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">

</xml_diff>